<commit_message>
varying texture size exp
</commit_message>
<xml_diff>
--- a/HW/HW2/report/fig/wes.xlsx
+++ b/HW/HW2/report/fig/wes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="799" firstSheet="1" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="799" firstSheet="15" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="TriArea" sheetId="1" r:id="rId1"/>
@@ -27,10 +27,11 @@
     <sheet name="TriAreaTStrip" sheetId="12" r:id="rId13"/>
     <sheet name="TriAreaIDTStrip" sheetId="16" r:id="rId14"/>
     <sheet name="TriAreaTStrip_IDTSrip Fig" sheetId="17" r:id="rId15"/>
-    <sheet name="textTest128" sheetId="18" r:id="rId16"/>
-    <sheet name="textTest16384" sheetId="19" r:id="rId17"/>
-    <sheet name="textTest Fig" sheetId="22" r:id="rId18"/>
-    <sheet name="bucketSize" sheetId="23" r:id="rId19"/>
+    <sheet name="textTest 2^7" sheetId="18" r:id="rId16"/>
+    <sheet name="textTest 2^14" sheetId="19" r:id="rId17"/>
+    <sheet name="textTest 2^7 Fig" sheetId="22" r:id="rId18"/>
+    <sheet name="textTest 2^14 Fig" sheetId="25" r:id="rId19"/>
+    <sheet name="bucketSize" sheetId="23" r:id="rId20"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -1120,6 +1121,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="819677792"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -2786,6 +2788,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="594780312"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -4315,6 +4318,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="819440792"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -5404,6 +5408,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="819442432"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -6819,6 +6824,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="819230472"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -9652,6 +9658,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="816102048"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -9759,10 +9766,1223 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.12497813739494261"/>
-          <c:y val="0.11301422704831533"/>
-          <c:w val="0.7264922591658719"/>
-          <c:h val="0.75339030763165415"/>
+          <c:x val="8.3925504479250929E-2"/>
+          <c:y val="5.8525224721449012E-2"/>
+          <c:w val="0.83352233783892515"/>
+          <c:h val="0.84016908911518207"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>MVerts/Sec - area =2^7 p</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'textTest 2^7'!$B$13:$B$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4096</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'textTest 2^7'!$C$13:$C$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>30.104369999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>29.255269999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>31.231180000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>27.721730000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>26.7178</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24.740659999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>19.161909999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.3167600000000004</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.4195799999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.1390099999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-EEC6-460B-917F-E0C0A4CD0DA2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>MTris/Sec - area =2^7 p</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'textTest 2^7'!$B$13:$B$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4096</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'textTest 2^7'!$E$13:$E$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>10.034790000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.7517600000000009</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.41039</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.2405799999999996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.9059299999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.2468899999999987</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.3872999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.1055900000000003</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.47319</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.3796700000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-EEC6-460B-917F-E0C0A4CD0DA2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="547723200"/>
+        <c:axId val="774397528"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:v>MVerts/Sec - area =2^14 p</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="25400" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:ln w="25400">
+                      <a:solidFill>
+                        <a:schemeClr val="accent1"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'textTest 2^14'!$B$13:$B$22</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="10"/>
+                      <c:pt idx="0">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>16</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>32</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>64</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>128</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>256</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>512</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>1024</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>2048</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>4096</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'textTest 2^14'!$C$13:$C$22</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="10"/>
+                      <c:pt idx="0">
+                        <c:v>444.7</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>436.77</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>356.96</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>273.18</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>240.67</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>214.59</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>115</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>47.89</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>35.880000000000003</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>26.65</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000000-EEC6-460B-917F-E0C0A4CD0DA2}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="2"/>
+                <c:order val="2"/>
+                <c:tx>
+                  <c:v>MTris/Sec - area =2^14 p</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="25400" cap="rnd">
+                    <a:solidFill>
+                      <a:srgbClr val="FF0000"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:srgbClr val="FF0000"/>
+                    </a:solidFill>
+                    <a:ln w="25400">
+                      <a:solidFill>
+                        <a:srgbClr val="FF0000"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'textTest 2^14'!$B$13:$B$22</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="10"/>
+                      <c:pt idx="0">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>16</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>32</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>64</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>128</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>256</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>512</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>1024</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>2048</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>4096</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'textTest 2^14'!$E$13:$E$22</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="10"/>
+                      <c:pt idx="0">
+                        <c:v>148.22999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>145.59</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>118.99</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>91.06</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>80.22</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>71.53</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>38.33</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>15.96</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>11.96</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>8.8800000000000008</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000002-EEC6-460B-917F-E0C0A4CD0DA2}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+          </c:ext>
+        </c:extLst>
+      </c:scatterChart>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>MFrags/Sec - area =2^7 p</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'textTest 2^7'!$B$13:$B$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4096</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'textTest 2^7'!$D$13:$D$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1284.45325</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1248.22488</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1332.5303799999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1182.79375</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1139.9593799999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1055.6015</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>817.57474999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>397.51515999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>188.56892000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>176.59767000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-EEC6-460B-917F-E0C0A4CD0DA2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="826291856"/>
+        <c:axId val="826299072"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="1"/>
+                <c:tx>
+                  <c:v>MFrags/Sec - area =2^14 p</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="25400" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent2"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent2"/>
+                    </a:solidFill>
+                    <a:ln w="25400">
+                      <a:solidFill>
+                        <a:schemeClr val="accent2"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'textTest 2^14'!$B$13:$B$22</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="10"/>
+                      <c:pt idx="0">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>16</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>32</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>64</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>128</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>256</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>512</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>1024</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>2048</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>4096</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'textTest 2^14'!$D$13:$D$22</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="10"/>
+                      <c:pt idx="0">
+                        <c:v>2428682</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2385346.5</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>1949477.63</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>1491953.25</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>1314390</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>1171947.5</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>628053.38</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>261541.78</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>195952.64000000001</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>145551.35999999999</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000001-EEC6-460B-917F-E0C0A4CD0DA2}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+          </c:ext>
+        </c:extLst>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="547723200"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:min val="7"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2400">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>Texture</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2400" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t> Size</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="2400">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.41601925456222782"/>
+              <c:y val="0.92476831050563535"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="2400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="774397528"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="774397528"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2400">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>Rate</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1800" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t> </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2000" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>(*10^3)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="547723200"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="826299072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="826291856"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="826291856"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="826299072"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.58011895796965407"/>
+          <c:y val="7.6044813509840187E-2"/>
+          <c:w val="0.35390636697936784"/>
+          <c:h val="0.26339147877177432"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1200" b="1"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.125633178562445E-2"/>
+          <c:y val="7.0633891905197088E-2"/>
+          <c:w val="0.7968682013070576"/>
+          <c:h val="0.79577064277477261"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -9800,7 +11020,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>textTest16384!$B$13:$B$22</c:f>
+              <c:f>'textTest 2^14'!$B$13:$B$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -9839,7 +11059,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>textTest16384!$C$13:$C$22</c:f>
+              <c:f>'textTest 2^14'!$C$13:$C$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -9879,7 +11099,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-EEC6-460B-917F-E0C0A4CD0DA2}"/>
+              <c16:uniqueId val="{00000000-2090-4803-82D6-3F8E124C58F1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -9915,7 +11135,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>textTest16384!$B$13:$B$22</c:f>
+              <c:f>'textTest 2^14'!$B$13:$B$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -9954,7 +11174,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>textTest16384!$E$13:$E$22</c:f>
+              <c:f>'textTest 2^14'!$E$13:$E$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -9994,239 +11214,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-EEC6-460B-917F-E0C0A4CD0DA2}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:v>MVerts/Sec - area =2^7 p</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:prstDash val="sysDash"/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>textTest128!$B$13:$B$22</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>256</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>512</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1024</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2048</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>4096</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>textTest128!$C$13:$C$22</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>30.104369999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>29.255269999999999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>31.231180000000002</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>27.721730000000001</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>26.7178</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>24.740659999999998</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>19.161909999999999</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>9.3167600000000004</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>4.4195799999999998</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>4.1390099999999999</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-EEC6-460B-917F-E0C0A4CD0DA2}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:v>MTris/Sec - area =2^7 p</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:prstDash val="sysDash"/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:ln w="25400">
-                <a:solidFill>
-                  <a:srgbClr val="FF0000"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>textTest128!$B$13:$B$22</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>256</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>512</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1024</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2048</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>4096</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>textTest128!$E$13:$E$22</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>10.034790000000001</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>9.7517600000000009</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10.41039</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9.2405799999999996</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>8.9059299999999997</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>8.2468899999999987</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6.3872999999999998</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3.1055900000000003</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.47319</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.3796700000000002</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-EEC6-460B-917F-E0C0A4CD0DA2}"/>
+              <c16:uniqueId val="{00000001-2090-4803-82D6-3F8E124C58F1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -10240,6 +11228,270 @@
         </c:dLbls>
         <c:axId val="547723200"/>
         <c:axId val="774397528"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="3"/>
+                <c:order val="3"/>
+                <c:tx>
+                  <c:v>MVerts/Sec - area =2^7 p</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="25400" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:prstDash val="sysDash"/>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:ln w="25400">
+                      <a:solidFill>
+                        <a:schemeClr val="accent1"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'textTest 2^7'!$B$13:$B$22</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="10"/>
+                      <c:pt idx="0">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>16</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>32</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>64</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>128</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>256</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>512</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>1024</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>2048</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>4096</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'textTest 2^7'!$C$13:$C$22</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="10"/>
+                      <c:pt idx="0">
+                        <c:v>30.104369999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>29.255269999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>31.231180000000002</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>27.721730000000001</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>26.7178</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>24.740659999999998</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>19.161909999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>9.3167600000000004</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>4.4195799999999998</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>4.1390099999999999</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000003-2090-4803-82D6-3F8E124C58F1}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="5"/>
+                <c:order val="5"/>
+                <c:tx>
+                  <c:v>MTris/Sec - area =2^7 p</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="25400" cap="rnd">
+                    <a:solidFill>
+                      <a:srgbClr val="FF0000"/>
+                    </a:solidFill>
+                    <a:prstDash val="sysDash"/>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:srgbClr val="FF0000"/>
+                    </a:solidFill>
+                    <a:ln w="25400">
+                      <a:solidFill>
+                        <a:srgbClr val="FF0000"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'textTest 2^7'!$B$13:$B$22</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="10"/>
+                      <c:pt idx="0">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>16</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>32</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>64</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>128</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>256</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>512</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>1024</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>2048</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>4096</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'textTest 2^7'!$E$13:$E$22</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="10"/>
+                      <c:pt idx="0">
+                        <c:v>10.034790000000001</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>9.7517600000000009</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>10.41039</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>9.2405799999999996</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>8.9059299999999997</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>8.2468899999999987</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>6.3872999999999998</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>3.1055900000000003</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>1.47319</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>1.3796700000000002</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="0"/>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000005-2090-4803-82D6-3F8E124C58F1}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+          </c:ext>
+        </c:extLst>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -10276,7 +11528,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>textTest16384!$B$13:$B$22</c:f>
+              <c:f>'textTest 2^14'!$B$13:$B$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -10315,7 +11567,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>textTest16384!$D$13:$D$22</c:f>
+              <c:f>'textTest 2^14'!$D$13:$D$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -10355,123 +11607,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-EEC6-460B-917F-E0C0A4CD0DA2}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:v>MFrags/Sec - area =2^7 p</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:prstDash val="sysDash"/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>textTest128!$B$13:$B$22</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>256</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>512</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1024</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2048</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>4096</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>textTest128!$D$13:$D$22</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1284.45325</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1248.22488</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1332.5303799999999</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1182.79375</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1139.9593799999998</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1055.6015</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>817.57474999999999</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>397.51515999999998</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>188.56892000000002</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>176.59767000000002</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-EEC6-460B-917F-E0C0A4CD0DA2}"/>
+              <c16:uniqueId val="{00000002-2090-4803-82D6-3F8E124C58F1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -10485,6 +11621,140 @@
         </c:dLbls>
         <c:axId val="826291856"/>
         <c:axId val="826299072"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="4"/>
+                <c:order val="4"/>
+                <c:tx>
+                  <c:v>MFrags/Sec - area =2^7 p</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="25400" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent2"/>
+                    </a:solidFill>
+                    <a:prstDash val="sysDash"/>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent2"/>
+                    </a:solidFill>
+                    <a:ln w="25400">
+                      <a:solidFill>
+                        <a:schemeClr val="accent2"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'textTest 2^7'!$B$13:$B$22</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="10"/>
+                      <c:pt idx="0">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>16</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>32</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>64</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>128</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>256</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>512</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>1024</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>2048</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>4096</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'textTest 2^7'!$D$13:$D$22</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="10"/>
+                      <c:pt idx="0">
+                        <c:v>1284.45325</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>1248.22488</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>1332.5303799999999</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>1182.79375</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>1139.9593799999998</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>1055.6015</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>817.57474999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>397.51515999999998</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>188.56892000000002</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>176.59767000000002</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000004-2090-4803-82D6-3F8E124C58F1}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+          </c:ext>
+        </c:extLst>
       </c:scatterChart>
       <c:valAx>
         <c:axId val="547723200"/>
@@ -10526,7 +11796,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1800">
+                  <a:rPr lang="en-US" sz="2400">
                     <a:solidFill>
                       <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
@@ -10536,7 +11806,7 @@
                   <a:t>Texture</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1800" baseline="0">
+                  <a:rPr lang="en-US" sz="2400" baseline="0">
                     <a:solidFill>
                       <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
@@ -10545,7 +11815,7 @@
                   </a:rPr>
                   <a:t> Size</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-US" sz="1800">
+                <a:endParaRPr lang="en-US" sz="2400">
                   <a:solidFill>
                     <a:sysClr val="windowText" lastClr="000000"/>
                   </a:solidFill>
@@ -10555,6 +11825,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.42812608699717886"/>
+              <c:y val="0.9066053097300133"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -10812,6 +12090,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="826299072"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -10828,9 +12107,9 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.53320166320886353"/>
-          <c:y val="7.6044813509840187E-2"/>
-          <c:w val="0.33924471236662079"/>
+          <c:x val="0.55079564874415998"/>
+          <c:y val="6.1918035128800772E-2"/>
+          <c:w val="0.34657553967299431"/>
           <c:h val="0.27751825715281375"/>
         </c:manualLayout>
       </c:layout>
@@ -10847,7 +12126,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
@@ -11212,6 +12491,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -14825,6 +16144,522 @@
 </file>
 
 <file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -15404,7 +17239,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -15428,10 +17263,23 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
+    <sheetView tabSelected="1" zoomScale="102" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
     <sheetView zoomScale="102" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </chartsheet>
 </file>
 
@@ -15604,7 +17452,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8663609" cy="6286500"/>
+    <xdr:ext cx="8667750" cy="6296025"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -15677,6 +17525,39 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{958068B0-AF24-4775-BB7C-B9A4E92D6158}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8662051" cy="6293013"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F61E12DF-EACE-40F1-B4D4-2D2A015DCCBD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -16815,7 +18696,7 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
pass on intro + prepare deliverable
</commit_message>
<xml_diff>
--- a/HW/HW2/report/fig/wes.xlsx
+++ b/HW/HW2/report/fig/wes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="799" firstSheet="20" activeTab="26"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="799" firstSheet="20" activeTab="22"/>
   </bookViews>
   <sheets>
     <sheet name="TriArea" sheetId="1" r:id="rId1"/>
@@ -2279,7 +2279,17 @@
   <c:chart>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.10384007205683736"/>
+          <c:y val="2.8253556762078833E-2"/>
+          <c:w val="0.87121306489652384"/>
+          <c:h val="0.94147477527855095"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
@@ -2290,7 +2300,7 @@
             <c:v>POW2</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="38100" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -2537,7 +2547,7 @@
             <c:v>Sqrt</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="38100" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
@@ -2784,9 +2794,9 @@
             <c:v>Log2</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="38100" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:srgbClr val="FF0000"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -3041,7 +3051,7 @@
           <c:orientation val="minMax"/>
           <c:max val="100"/>
         </c:scaling>
-        <c:delete val="0"/>
+        <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
@@ -3061,39 +3071,6 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
         <c:crossAx val="508061928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
@@ -3141,16 +3118,13 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -3174,9 +3148,9 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.91313510712604362"/>
-          <c:y val="0.44874379887516369"/>
-          <c:w val="7.8057305033004759E-2"/>
+          <c:x val="0.39411254909489674"/>
+          <c:y val="7.5393297296541414E-2"/>
+          <c:w val="0.22760614085509309"/>
           <c:h val="0.21793296582856148"/>
         </c:manualLayout>
       </c:layout>
@@ -3193,16 +3167,13 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
@@ -3257,7 +3228,17 @@
   <c:chart>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.11566706314705374"/>
+          <c:y val="2.5736002770056252E-2"/>
+          <c:w val="0.863813893499357"/>
+          <c:h val="0.94852799445988745"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
@@ -3268,9 +3249,9 @@
             <c:v>POW2</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="38100" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="FF0000"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -3515,7 +3496,7 @@
             <c:v>Log2</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="38100" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent3"/>
               </a:solidFill>
@@ -3762,7 +3743,7 @@
             <c:v>Cos</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="38100" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent4"/>
               </a:solidFill>
@@ -4009,7 +3990,7 @@
             <c:v>Sin</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="38100" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent5"/>
               </a:solidFill>
@@ -4531,7 +4512,7 @@
           <c:orientation val="minMax"/>
           <c:max val="100"/>
         </c:scaling>
-        <c:delete val="0"/>
+        <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
@@ -4551,39 +4532,6 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
         <c:crossAx val="508061928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
@@ -4632,16 +4580,13 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -4665,10 +4610,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.91313510712604362"/>
-          <c:y val="0.44874379887516369"/>
-          <c:w val="7.8057305033004759E-2"/>
-          <c:h val="0.13668320299956346"/>
+          <c:x val="0.39997721093999561"/>
+          <c:y val="6.1266518915502E-2"/>
+          <c:w val="0.16162869509773148"/>
+          <c:h val="0.19319028897604371"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -4684,16 +4629,13 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
@@ -24006,7 +23948,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="117" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -24030,7 +23972,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>